<commit_message>
initial change of toplevel
</commit_message>
<xml_diff>
--- a/cmip6/models/emac-2-53-aerchem/cmip6_messy-consortium_emac-2-53-aerchem_toplevel.xlsx
+++ b/cmip6/models/emac-2-53-aerchem/cmip6_messy-consortium_emac-2-53-aerchem_toplevel.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="1. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="2. Radiative Forcings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="425">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1271,12 +1271,33 @@
   </si>
   <si>
     <t>cmip6.toplevel.radiative_forcings.other.solar.additional_information</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>EMAC</t>
+  </si>
+  <si>
+    <t>2.54.0p3</t>
+  </si>
+  <si>
+    <t>Fortan, C</t>
+  </si>
+  <si>
+    <t>Modular Earth Submodel System</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>MESSy submodel A2O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -1469,17 +1490,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1517,7 +1543,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1551,6 +1577,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1585,9 +1612,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1760,24 +1788,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1785,7 +1813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1793,7 +1821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1801,7 +1829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1809,7 +1837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1817,12 +1845,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1838,7 +1866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="18">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1846,7 +1874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="18">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1854,13 +1882,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20.25">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20.25">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1876,19 +1904,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="80.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -1899,7 +1929,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1915,7 +1945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
@@ -1923,11 +1953,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="18">
       <c r="A9" s="11"/>
       <c r="B9" s="11"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
@@ -1943,7 +1973,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="15.75">
       <c r="A16" s="10" t="s">
         <v>27</v>
       </c>
@@ -1951,7 +1981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="18">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
     </row>
@@ -1973,12 +2003,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD224"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -2019,7 +2051,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -2072,7 +2106,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
+    <row r="16" spans="1:3" ht="177.95" customHeight="1">
       <c r="B16" s="11"/>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1">
@@ -2112,8 +2146,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="178" customHeight="1">
-      <c r="B25" s="11"/>
+    <row r="25" spans="1:3" ht="177.95" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
@@ -2148,7 +2184,9 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
+      <c r="B33" s="11">
+        <v>2018</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
@@ -2218,7 +2256,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="178" customHeight="1">
+    <row r="46" spans="1:3" ht="177.95" customHeight="1">
       <c r="B46" s="11"/>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1">
@@ -2298,7 +2336,9 @@
       </c>
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
-      <c r="B62" s="11"/>
+      <c r="B62" s="11" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="24" customHeight="1">
       <c r="A64" s="9" t="s">
@@ -2325,7 +2365,9 @@
       </c>
     </row>
     <row r="67" spans="1:34" ht="24" customHeight="1">
-      <c r="B67" s="11"/>
+      <c r="B67" s="11" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="69" spans="1:34" ht="24" customHeight="1">
       <c r="A69" s="9" t="s">
@@ -2347,7 +2389,9 @@
       </c>
     </row>
     <row r="71" spans="1:34" ht="24" customHeight="1">
-      <c r="B71" s="11"/>
+      <c r="B71" s="11" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="73" spans="1:34" ht="24" customHeight="1">
       <c r="A73" s="9" t="s">
@@ -2369,7 +2413,9 @@
       </c>
     </row>
     <row r="75" spans="1:34" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
+      <c r="B75" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="AA75" s="6" t="s">
         <v>104</v>
       </c>
@@ -2426,7 +2472,9 @@
       </c>
     </row>
     <row r="83" spans="1:30" ht="24" customHeight="1">
-      <c r="B83" s="11"/>
+      <c r="B83" s="11" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="85" spans="1:30" ht="24" customHeight="1">
       <c r="A85" s="9" t="s">
@@ -2448,7 +2496,12 @@
       </c>
     </row>
     <row r="87" spans="1:30" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+      <c r="B87" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>424</v>
+      </c>
       <c r="AA87" s="6" t="s">
         <v>123</v>
       </c>
@@ -2521,7 +2574,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="178" customHeight="1">
+    <row r="100" spans="1:3" ht="177.95" customHeight="1">
       <c r="B100" s="11"/>
     </row>
     <row r="102" spans="1:3" ht="24" customHeight="1">
@@ -2686,7 +2739,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="178" customHeight="1">
+    <row r="132" spans="1:3" ht="177.95" customHeight="1">
       <c r="B132" s="11"/>
     </row>
     <row r="134" spans="1:3" ht="24" customHeight="1">
@@ -2713,7 +2766,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="178" customHeight="1">
+    <row r="137" spans="1:3" ht="177.95" customHeight="1">
       <c r="B137" s="11"/>
     </row>
     <row r="139" spans="1:3" ht="24" customHeight="1">
@@ -2740,7 +2793,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="178" customHeight="1">
+    <row r="142" spans="1:3" ht="177.95" customHeight="1">
       <c r="B142" s="11"/>
     </row>
     <row r="144" spans="1:3" ht="24" customHeight="1">
@@ -2767,7 +2820,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="178" customHeight="1">
+    <row r="147" spans="1:3" ht="177.95" customHeight="1">
       <c r="B147" s="11"/>
     </row>
     <row r="149" spans="1:3" ht="24" customHeight="1">
@@ -2794,7 +2847,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="178" customHeight="1">
+    <row r="152" spans="1:3" ht="177.95" customHeight="1">
       <c r="B152" s="11"/>
     </row>
     <row r="154" spans="1:3" ht="24" customHeight="1">
@@ -2821,7 +2874,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="178" customHeight="1">
+    <row r="157" spans="1:3" ht="177.95" customHeight="1">
       <c r="B157" s="11"/>
     </row>
     <row r="160" spans="1:3" ht="24" customHeight="1">
@@ -2861,7 +2914,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="178" customHeight="1">
+    <row r="166" spans="1:3" ht="177.95" customHeight="1">
       <c r="B166" s="11"/>
     </row>
     <row r="168" spans="1:3" ht="24" customHeight="1">
@@ -2888,7 +2941,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="178" customHeight="1">
+    <row r="171" spans="1:3" ht="177.95" customHeight="1">
       <c r="B171" s="11"/>
     </row>
     <row r="173" spans="1:3" ht="24" customHeight="1">
@@ -2915,7 +2968,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="178" customHeight="1">
+    <row r="176" spans="1:3" ht="177.95" customHeight="1">
       <c r="B176" s="11"/>
     </row>
     <row r="178" spans="1:3" ht="24" customHeight="1">
@@ -2942,7 +2995,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="178" customHeight="1">
+    <row r="181" spans="1:3" ht="177.95" customHeight="1">
       <c r="B181" s="11"/>
     </row>
     <row r="183" spans="1:3" ht="24" customHeight="1">
@@ -2969,7 +3022,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="178" customHeight="1">
+    <row r="186" spans="1:3" ht="177.95" customHeight="1">
       <c r="B186" s="11"/>
     </row>
     <row r="188" spans="1:3" ht="24" customHeight="1">
@@ -2996,7 +3049,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="178" customHeight="1">
+    <row r="191" spans="1:3" ht="177.95" customHeight="1">
       <c r="B191" s="11"/>
     </row>
     <row r="193" spans="1:3" ht="24" customHeight="1">
@@ -3023,7 +3076,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="178" customHeight="1">
+    <row r="196" spans="1:3" ht="177.95" customHeight="1">
       <c r="B196" s="11"/>
     </row>
     <row r="198" spans="1:3" ht="24" customHeight="1">
@@ -3050,7 +3103,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="178" customHeight="1">
+    <row r="201" spans="1:3" ht="177.95" customHeight="1">
       <c r="B201" s="11"/>
     </row>
     <row r="203" spans="1:3" ht="24" customHeight="1">
@@ -3077,7 +3130,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="178" customHeight="1">
+    <row r="206" spans="1:3" ht="177.95" customHeight="1">
       <c r="B206" s="11"/>
     </row>
     <row r="209" spans="1:3" ht="24" customHeight="1">
@@ -3117,7 +3170,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="178" customHeight="1">
+    <row r="215" spans="1:3" ht="177.95" customHeight="1">
       <c r="B215" s="11"/>
     </row>
     <row r="218" spans="1:3" ht="24" customHeight="1">
@@ -3157,7 +3210,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="178" customHeight="1">
+    <row r="224" spans="1:3" ht="177.95" customHeight="1">
       <c r="B224" s="11"/>
     </row>
   </sheetData>
@@ -3180,12 +3233,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD299"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG299"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="150.7109375" customWidth="1"/>
@@ -3252,7 +3307,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="177.95" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -3340,7 +3395,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="178" customHeight="1">
+    <row r="25" spans="1:33" ht="177.95" customHeight="1">
       <c r="B25" s="11"/>
     </row>
     <row r="28" spans="1:33" ht="24" customHeight="1">
@@ -3428,7 +3483,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="178" customHeight="1">
+    <row r="39" spans="1:33" ht="177.95" customHeight="1">
       <c r="B39" s="11"/>
     </row>
     <row r="42" spans="1:33" ht="24" customHeight="1">
@@ -3516,7 +3571,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="178" customHeight="1">
+    <row r="53" spans="1:33" ht="177.95" customHeight="1">
       <c r="B53" s="11"/>
     </row>
     <row r="56" spans="1:33" ht="24" customHeight="1">
@@ -3604,7 +3659,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="178" customHeight="1">
+    <row r="67" spans="1:33" ht="177.95" customHeight="1">
       <c r="B67" s="11"/>
     </row>
     <row r="70" spans="1:33" ht="24" customHeight="1">
@@ -3692,7 +3747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="178" customHeight="1">
+    <row r="81" spans="1:33" ht="177.95" customHeight="1">
       <c r="B81" s="11"/>
     </row>
     <row r="84" spans="1:33" ht="24" customHeight="1">
@@ -3817,7 +3872,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="178" customHeight="1">
+    <row r="99" spans="1:33" ht="177.95" customHeight="1">
       <c r="B99" s="11"/>
     </row>
     <row r="102" spans="1:33" ht="24" customHeight="1">
@@ -3905,7 +3960,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="113" spans="1:33" ht="178" customHeight="1">
+    <row r="113" spans="1:33" ht="177.95" customHeight="1">
       <c r="B113" s="11"/>
     </row>
     <row r="116" spans="1:33" ht="24" customHeight="1">
@@ -3993,7 +4048,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:33" ht="178" customHeight="1">
+    <row r="127" spans="1:33" ht="177.95" customHeight="1">
       <c r="B127" s="11"/>
     </row>
     <row r="130" spans="1:33" ht="24" customHeight="1">
@@ -4081,7 +4136,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="1:33" ht="178" customHeight="1">
+    <row r="141" spans="1:33" ht="177.95" customHeight="1">
       <c r="B141" s="11"/>
     </row>
     <row r="144" spans="1:33" ht="24" customHeight="1">
@@ -4169,7 +4224,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="1:33" ht="178" customHeight="1">
+    <row r="155" spans="1:33" ht="177.95" customHeight="1">
       <c r="B155" s="11"/>
     </row>
     <row r="158" spans="1:33" ht="24" customHeight="1">
@@ -4279,7 +4334,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="173" spans="1:33" ht="178" customHeight="1">
+    <row r="173" spans="1:33" ht="177.95" customHeight="1">
       <c r="B173" s="11"/>
     </row>
     <row r="176" spans="1:33" ht="24" customHeight="1">
@@ -4411,7 +4466,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="195" spans="1:33" ht="178" customHeight="1">
+    <row r="195" spans="1:33" ht="177.95" customHeight="1">
       <c r="B195" s="11"/>
     </row>
     <row r="198" spans="1:33" ht="24" customHeight="1">
@@ -4499,7 +4554,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="209" spans="1:33" ht="178" customHeight="1">
+    <row r="209" spans="1:33" ht="177.95" customHeight="1">
       <c r="B209" s="11"/>
     </row>
     <row r="212" spans="1:33" ht="24" customHeight="1">
@@ -4667,7 +4722,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="231" spans="1:33" ht="178" customHeight="1">
+    <row r="231" spans="1:33" ht="177.95" customHeight="1">
       <c r="B231" s="11"/>
     </row>
     <row r="234" spans="1:33" ht="24" customHeight="1">
@@ -4835,7 +4890,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="253" spans="1:32" ht="178" customHeight="1">
+    <row r="253" spans="1:32" ht="177.95" customHeight="1">
       <c r="B253" s="11"/>
     </row>
     <row r="256" spans="1:32" ht="24" customHeight="1">
@@ -4923,7 +4978,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="267" spans="1:33" ht="178" customHeight="1">
+    <row r="267" spans="1:33" ht="177.95" customHeight="1">
       <c r="B267" s="11"/>
     </row>
     <row r="270" spans="1:33" ht="24" customHeight="1">
@@ -5033,7 +5088,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="285" spans="1:33" ht="178" customHeight="1">
+    <row r="285" spans="1:33" ht="177.95" customHeight="1">
       <c r="B285" s="11"/>
     </row>
     <row r="288" spans="1:33" ht="24" customHeight="1">
@@ -5118,7 +5173,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="299" spans="1:32" ht="178" customHeight="1">
+    <row r="299" spans="1:32" ht="177.95" customHeight="1">
       <c r="B299" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
long version of model name
</commit_message>
<xml_diff>
--- a/cmip6/models/emac-2-53-aerchem/cmip6_messy-consortium_emac-2-53-aerchem_toplevel.xlsx
+++ b/cmip6/models/emac-2-53-aerchem/cmip6_messy-consortium_emac-2-53-aerchem_toplevel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -1276,9 +1276,6 @@
     <t>No.</t>
   </si>
   <si>
-    <t>EMAC</t>
-  </si>
-  <si>
     <t>2.54.0p3</t>
   </si>
   <si>
@@ -1292,6 +1289,9 @@
   </si>
   <si>
     <t>MESSy submodel A2O</t>
+  </si>
+  <si>
+    <t>ECHAM/MESSy Atmospheric Chemistry (EMAC)</t>
   </si>
 </sst>
 </file>
@@ -2006,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
       <c r="B6" s="11" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
@@ -2337,7 +2337,7 @@
     </row>
     <row r="62" spans="1:3" ht="24" customHeight="1">
       <c r="B62" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="24" customHeight="1">
@@ -2366,7 +2366,7 @@
     </row>
     <row r="67" spans="1:34" ht="24" customHeight="1">
       <c r="B67" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="69" spans="1:34" ht="24" customHeight="1">
@@ -2390,7 +2390,7 @@
     </row>
     <row r="71" spans="1:34" ht="24" customHeight="1">
       <c r="B71" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="73" spans="1:34" ht="24" customHeight="1">
@@ -2473,7 +2473,7 @@
     </row>
     <row r="83" spans="1:30" ht="24" customHeight="1">
       <c r="B83" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="85" spans="1:30" ht="24" customHeight="1">
@@ -2500,7 +2500,7 @@
         <v>111</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AA87" s="6" t="s">
         <v>123</v>
@@ -3236,7 +3236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>